<commit_message>
items and fix spawner
</commit_message>
<xml_diff>
--- a/INFO D.xlsx
+++ b/INFO D.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kelvin\Documents\GitHub\Craft-to-Exile-Dissonance-Server\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kelvin Vuu\Documents\GitHub\Craft-to-Exile-Dissonance-Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF82195A-7A69-4C6B-954B-77E39D1813D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443FBD0A-C61A-4B14-B883-81348F274C04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1005" yWindow="2295" windowWidth="28800" windowHeight="15885" tabRatio="680" firstSheet="10" activeTab="13" xr2:uid="{52F6E08D-EA9B-4E8E-A88E-E860D0D32EA0}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" tabRatio="680" firstSheet="1" activeTab="13" xr2:uid="{52F6E08D-EA9B-4E8E-A88E-E860D0D32EA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Overworld" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3843" uniqueCount="2154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3865" uniqueCount="2166">
   <si>
     <t>Quest</t>
   </si>
@@ -6514,6 +6514,42 @@
   </si>
   <si>
     <t>high_magic_shield_flat</t>
+  </si>
+  <si>
+    <t>Ano, Cen</t>
+  </si>
+  <si>
+    <t>Holy</t>
+  </si>
+  <si>
+    <t>increase_healing</t>
+  </si>
+  <si>
+    <t>Goh, Ano, Ita</t>
+  </si>
+  <si>
+    <t>low_health_percent</t>
+  </si>
+  <si>
+    <t>Heart</t>
+  </si>
+  <si>
+    <t>Paladin</t>
+  </si>
+  <si>
+    <t>Rah, Goh, Mos, Ano</t>
+  </si>
+  <si>
+    <t>Healer's Robes</t>
+  </si>
+  <si>
+    <t>Angel's Garbs</t>
+  </si>
+  <si>
+    <t>mana_precent</t>
+  </si>
+  <si>
+    <t>low_increase_healing_flat</t>
   </si>
 </sst>
 </file>
@@ -23032,10 +23068,10 @@
   <sheetPr>
     <tabColor theme="2" tint="-9.9978637043366805E-2"/>
   </sheetPr>
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24102,7 +24138,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>758</v>
       </c>
@@ -24134,7 +24170,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>760</v>
       </c>
@@ -24166,7 +24202,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>762</v>
       </c>
@@ -24195,7 +24231,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>2134</v>
       </c>
@@ -24227,7 +24263,7 @@
         <v>2139</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>2140</v>
       </c>
@@ -24259,7 +24295,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>2143</v>
       </c>
@@ -24288,7 +24324,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>2144</v>
       </c>
@@ -24317,62 +24353,156 @@
         <v>2151</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>2145</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="2">
         <v>0</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="2">
         <v>1</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="2">
         <v>6666</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="2">
         <v>3</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" s="2" t="s">
         <v>2149</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G40" s="2" t="s">
         <v>792</v>
       </c>
-      <c r="H40" t="s">
+      <c r="H40" s="2" t="s">
         <v>733</v>
       </c>
-      <c r="I40" t="s">
+      <c r="I40" s="2" t="s">
         <v>629</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>2146</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="2">
         <v>0</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="2">
         <v>1</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="2">
         <v>6666</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="2">
         <v>3</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="2" t="s">
         <v>2150</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G41" s="2" t="s">
         <v>790</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H41" s="2" t="s">
         <v>621</v>
       </c>
-      <c r="I41" t="s">
+      <c r="I41" s="2" t="s">
         <v>732</v>
+      </c>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
+        <v>2155</v>
+      </c>
+      <c r="B42" s="8">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>6666</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="F42" t="s">
+        <v>2154</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>2156</v>
+      </c>
+      <c r="H42" s="8" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
+        <v>2159</v>
+      </c>
+      <c r="B43" s="8">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>6666</v>
+      </c>
+      <c r="E43">
+        <v>3</v>
+      </c>
+      <c r="F43" t="s">
+        <v>2157</v>
+      </c>
+      <c r="G43" s="8" t="s">
+        <v>2158</v>
+      </c>
+      <c r="H43" s="8" t="s">
+        <v>2165</v>
+      </c>
+      <c r="I43" s="8" t="s">
+        <v>2131</v>
+      </c>
+      <c r="J43" s="8"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
+        <v>2160</v>
+      </c>
+      <c r="B44" s="8">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>4</v>
+      </c>
+      <c r="D44">
+        <v>75</v>
+      </c>
+      <c r="E44">
+        <v>4</v>
+      </c>
+      <c r="F44" t="s">
+        <v>2161</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>621</v>
+      </c>
+      <c r="H44" s="8" t="s">
+        <v>796</v>
+      </c>
+      <c r="I44" s="8" t="s">
+        <v>691</v>
+      </c>
+      <c r="J44" s="8" t="s">
+        <v>1075</v>
       </c>
     </row>
   </sheetData>
@@ -24385,10 +24515,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:N42"/>
+  <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25856,39 +25986,111 @@
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="A42" s="2" t="s">
         <v>1690</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="2">
         <v>0</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="2">
         <v>1</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="2">
         <v>10000</v>
       </c>
-      <c r="E42" s="17">
+      <c r="E42" s="9">
         <v>20</v>
       </c>
-      <c r="F42" s="17">
+      <c r="F42" s="9">
         <v>50</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="2">
         <v>4</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H42" s="2" t="s">
         <v>1693</v>
       </c>
-      <c r="I42" t="s">
+      <c r="I42" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="J42" t="s">
+      <c r="J42" s="2" t="s">
         <v>859</v>
       </c>
-      <c r="K42" t="s">
+      <c r="K42" s="2" t="s">
         <v>692</v>
       </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
+        <v>2162</v>
+      </c>
+      <c r="B43" s="8">
+        <v>0</v>
+      </c>
+      <c r="C43" s="8">
+        <v>1</v>
+      </c>
+      <c r="D43" s="8">
+        <v>10000</v>
+      </c>
+      <c r="E43" s="13">
+        <v>0</v>
+      </c>
+      <c r="F43" s="13">
+        <v>20</v>
+      </c>
+      <c r="G43" s="8">
+        <v>2</v>
+      </c>
+      <c r="H43" s="8" t="s">
+        <v>777</v>
+      </c>
+      <c r="I43" s="8" t="s">
+        <v>796</v>
+      </c>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
+        <v>2163</v>
+      </c>
+      <c r="B44" s="8">
+        <v>0</v>
+      </c>
+      <c r="C44" s="8">
+        <v>1</v>
+      </c>
+      <c r="D44" s="8">
+        <v>10000</v>
+      </c>
+      <c r="E44" s="13">
+        <v>15</v>
+      </c>
+      <c r="F44" s="13">
+        <v>50</v>
+      </c>
+      <c r="G44" s="8">
+        <v>3</v>
+      </c>
+      <c r="H44" s="8" t="s">
+        <v>777</v>
+      </c>
+      <c r="I44" s="8" t="s">
+        <v>2164</v>
+      </c>
+      <c r="J44" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -25904,7 +26106,7 @@
   <dimension ref="A1:P158"/>
   <sheetViews>
     <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="L39" sqref="L39"/>
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32328,7 +32530,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:H36"/>
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update uniques and fix bees
</commit_message>
<xml_diff>
--- a/INFO D.xlsx
+++ b/INFO D.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kelvin Vuu\Documents\GitHub\Craft-to-Exile-Dissonance-Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149D528F-4476-4215-A99A-92FDCA260380}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C29E44AA-1CED-4B33-B128-E434056C4DEA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" tabRatio="680" firstSheet="3" activeTab="14" xr2:uid="{52F6E08D-EA9B-4E8E-A88E-E860D0D32EA0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="680" firstSheet="3" activeTab="14" xr2:uid="{52F6E08D-EA9B-4E8E-A88E-E860D0D32EA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Overworld" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3901" uniqueCount="2192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3910" uniqueCount="2197">
   <si>
     <t>Quest</t>
   </si>
@@ -6631,6 +6631,21 @@
   </si>
   <si>
     <t>high_block_strength_percent</t>
+  </si>
+  <si>
+    <t>ctecu:vessel_of_charisma</t>
+  </si>
+  <si>
+    <t>vessel_of_charisma</t>
+  </si>
+  <si>
+    <t>crippled_health_percent</t>
+  </si>
+  <si>
+    <t>crippled_magic_shield_percent</t>
+  </si>
+  <si>
+    <t>very_high_spell_damage_flat</t>
   </si>
 </sst>
 </file>
@@ -26184,10 +26199,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:P160"/>
+  <dimension ref="A1:P161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="I143" sqref="I143"/>
+    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="E138" sqref="E138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32050,6 +32065,44 @@
       <c r="O160" s="2"/>
       <c r="P160" s="2" t="s">
         <v>884</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A161" s="8" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B161" t="s">
+        <v>2192</v>
+      </c>
+      <c r="C161" s="13" t="s">
+        <v>2193</v>
+      </c>
+      <c r="D161" s="13">
+        <v>4</v>
+      </c>
+      <c r="E161" s="13">
+        <v>3</v>
+      </c>
+      <c r="F161" s="13">
+        <v>250</v>
+      </c>
+      <c r="G161" s="8" t="s">
+        <v>1057</v>
+      </c>
+      <c r="I161" t="s">
+        <v>2194</v>
+      </c>
+      <c r="J161" t="s">
+        <v>2195</v>
+      </c>
+      <c r="K161" t="s">
+        <v>800</v>
+      </c>
+      <c r="L161" t="s">
+        <v>2196</v>
+      </c>
+      <c r="M161" t="s">
+        <v>2184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove serene, fix some bugs, new sets
</commit_message>
<xml_diff>
--- a/INFO D.xlsx
+++ b/INFO D.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kelvin Vuu\Documents\GitHub\Craft-to-Exile-Dissonance-Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5E10C8-7250-4A4F-AB69-D040BC7B5B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00CA05CD-0C1A-47BC-9182-F185EDD216B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="680" firstSheet="3" activeTab="13" xr2:uid="{52F6E08D-EA9B-4E8E-A88E-E860D0D32EA0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="680" firstSheet="4" activeTab="13" xr2:uid="{52F6E08D-EA9B-4E8E-A88E-E860D0D32EA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Overworld" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,7 @@
     <sheet name="MineColonies Research" sheetId="23" r:id="rId20"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">Sets!$A$1:$N$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">Uniques!$A$1:$P$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3931" uniqueCount="2209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3954" uniqueCount="2221">
   <si>
     <t>Quest</t>
   </si>
@@ -6682,13 +6683,49 @@
   </si>
   <si>
     <t>major_all_dot_dmg_flat</t>
+  </si>
+  <si>
+    <t>plate + shield</t>
+  </si>
+  <si>
+    <t>very_high_block_strength_flat</t>
+  </si>
+  <si>
+    <t>Orphan's Call</t>
+  </si>
+  <si>
+    <t>Naj's Ancient Vestige</t>
+  </si>
+  <si>
+    <t>mana_battery_trait_flat</t>
+  </si>
+  <si>
+    <t>The Disciple</t>
+  </si>
+  <si>
+    <t>Hsarus' Defense</t>
+  </si>
+  <si>
+    <t>high_block_strength_flat</t>
+  </si>
+  <si>
+    <t>major_armor_percent</t>
+  </si>
+  <si>
+    <t>Death's Disguise</t>
+  </si>
+  <si>
+    <t>much_less_mana_percent</t>
+  </si>
+  <si>
+    <t>high_physical_thorns_reflect_flat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6743,6 +6780,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -6938,7 +6982,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -7001,6 +7045,7 @@
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -23202,7 +23247,7 @@
   </sheetPr>
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="G18" sqref="G18:I18"/>
     </sheetView>
   </sheetViews>
@@ -24711,10 +24756,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:N46"/>
+  <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24852,40 +24897,39 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>778</v>
-      </c>
-      <c r="B5" s="17">
+      <c r="A5" s="8" t="s">
+        <v>2152</v>
+      </c>
+      <c r="B5" s="8">
         <v>0</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="8">
         <v>1</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="8">
         <v>10000</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="13">
         <v>0</v>
       </c>
-      <c r="F5" s="17">
-        <v>25</v>
-      </c>
-      <c r="G5" s="17">
-        <v>3</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>779</v>
-      </c>
-      <c r="I5" t="s">
-        <v>697</v>
-      </c>
-      <c r="J5" t="s">
-        <v>705</v>
-      </c>
+      <c r="F5" s="13">
+        <v>20</v>
+      </c>
+      <c r="G5" s="8">
+        <v>2</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>777</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>796</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="B6" s="17">
         <v>0</v>
@@ -24900,21 +24944,24 @@
         <v>0</v>
       </c>
       <c r="F6" s="17">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G6" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="I6" t="s">
-        <v>621</v>
+        <v>697</v>
+      </c>
+      <c r="J6" t="s">
+        <v>705</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>726</v>
+        <v>780</v>
       </c>
       <c r="B7" s="17">
         <v>0</v>
@@ -24929,7 +24976,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="17">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G7" s="17">
         <v>2</v>
@@ -24938,105 +24985,105 @@
         <v>781</v>
       </c>
       <c r="I7" t="s">
-        <v>628</v>
+        <v>621</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>782</v>
-      </c>
-      <c r="B8">
+      <c r="A8" s="17" t="s">
+        <v>726</v>
+      </c>
+      <c r="B8" s="17">
         <v>0</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="17">
         <v>1</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="17">
         <v>10000</v>
       </c>
       <c r="E8" s="17">
         <v>0</v>
       </c>
       <c r="F8" s="17">
-        <v>100</v>
-      </c>
-      <c r="G8">
+        <v>35</v>
+      </c>
+      <c r="G8" s="17">
         <v>2</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="17" t="s">
+        <v>781</v>
+      </c>
+      <c r="I8" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>782</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9" s="62">
+        <v>2</v>
+      </c>
+      <c r="D9" s="62">
+        <v>2500</v>
+      </c>
+      <c r="E9" s="17">
+        <v>0</v>
+      </c>
+      <c r="F9" s="62">
+        <v>50</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9" t="s">
         <v>783</v>
       </c>
-      <c r="I8" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>785</v>
-      </c>
-      <c r="B9" s="17">
+      <c r="I9" s="62" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1679</v>
+      </c>
+      <c r="B10">
         <v>0</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C10">
         <v>1</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D10">
         <v>10000</v>
       </c>
-      <c r="E9" s="17">
-        <v>10</v>
-      </c>
-      <c r="F9" s="17">
-        <v>30</v>
-      </c>
-      <c r="G9" s="17">
-        <v>3</v>
-      </c>
-      <c r="H9" s="17" t="s">
-        <v>786</v>
-      </c>
-      <c r="I9" t="s">
-        <v>787</v>
-      </c>
-      <c r="J9" t="s">
-        <v>788</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>789</v>
-      </c>
-      <c r="B10" s="17">
-        <v>0</v>
-      </c>
-      <c r="C10" s="17">
-        <v>1</v>
-      </c>
-      <c r="D10" s="17">
-        <v>10000</v>
-      </c>
       <c r="E10" s="17">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F10" s="17">
-        <v>30</v>
-      </c>
-      <c r="G10" s="17">
-        <v>3</v>
-      </c>
-      <c r="H10" s="17" t="s">
-        <v>786</v>
+        <v>35</v>
+      </c>
+      <c r="G10">
+        <v>4</v>
+      </c>
+      <c r="H10" t="s">
+        <v>1681</v>
       </c>
       <c r="I10" t="s">
-        <v>621</v>
+        <v>805</v>
       </c>
       <c r="J10" t="s">
-        <v>790</v>
+        <v>800</v>
+      </c>
+      <c r="K10" t="s">
+        <v>1682</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>791</v>
+        <v>785</v>
       </c>
       <c r="B11" s="17">
         <v>0</v>
@@ -25059,28 +25106,24 @@
       <c r="H11" s="17" t="s">
         <v>786</v>
       </c>
-      <c r="I11" s="17" t="s">
-        <v>711</v>
-      </c>
-      <c r="J11" s="17" t="s">
-        <v>792</v>
-      </c>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
+      <c r="I11" t="s">
+        <v>787</v>
+      </c>
+      <c r="J11" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>793</v>
-      </c>
-      <c r="B12">
+      <c r="A12" s="17" t="s">
+        <v>789</v>
+      </c>
+      <c r="B12" s="17">
         <v>0</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="17">
         <v>1</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="17">
         <v>10000</v>
       </c>
       <c r="E12" s="17">
@@ -25095,52 +25138,52 @@
       <c r="H12" s="17" t="s">
         <v>786</v>
       </c>
-      <c r="I12" s="17" t="s">
-        <v>717</v>
-      </c>
-      <c r="J12" s="17" t="s">
-        <v>794</v>
-      </c>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
+      <c r="I12" t="s">
+        <v>621</v>
+      </c>
+      <c r="J12" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>795</v>
-      </c>
-      <c r="B13">
+      <c r="A13" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="B13" s="17">
         <v>0</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="17">
         <v>1</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="17">
         <v>10000</v>
       </c>
       <c r="E13" s="17">
         <v>10</v>
       </c>
       <c r="F13" s="17">
-        <v>40</v>
-      </c>
-      <c r="G13">
+        <v>30</v>
+      </c>
+      <c r="G13" s="17">
         <v>3</v>
       </c>
-      <c r="H13" t="s">
-        <v>777</v>
-      </c>
-      <c r="I13" t="s">
-        <v>721</v>
-      </c>
-      <c r="J13" t="s">
-        <v>796</v>
-      </c>
+      <c r="H13" s="17" t="s">
+        <v>786</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>711</v>
+      </c>
+      <c r="J13" s="17" t="s">
+        <v>792</v>
+      </c>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -25155,30 +25198,28 @@
         <v>10</v>
       </c>
       <c r="F14" s="17">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="G14" s="17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>798</v>
+        <v>786</v>
       </c>
       <c r="I14" s="17" t="s">
-        <v>787</v>
+        <v>717</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>643</v>
-      </c>
-      <c r="K14" s="17" t="s">
-        <v>642</v>
-      </c>
+        <v>794</v>
+      </c>
+      <c r="K14" s="17"/>
       <c r="L14" s="17"/>
       <c r="M14" s="17"/>
       <c r="N14" s="17"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -25190,71 +25231,67 @@
         <v>10000</v>
       </c>
       <c r="E15" s="17">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F15" s="17">
-        <v>50</v>
-      </c>
-      <c r="G15" s="17">
-        <v>4</v>
-      </c>
-      <c r="H15" s="17" t="s">
-        <v>775</v>
-      </c>
-      <c r="I15" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15">
+        <v>3</v>
+      </c>
+      <c r="H15" t="s">
+        <v>777</v>
+      </c>
+      <c r="I15" t="s">
         <v>721</v>
       </c>
-      <c r="J15" s="17" t="s">
-        <v>661</v>
-      </c>
-      <c r="K15" s="17" t="s">
-        <v>800</v>
-      </c>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
+      <c r="J15" t="s">
+        <v>796</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>10000</v>
+      <c r="C16" s="62">
+        <v>2</v>
+      </c>
+      <c r="D16" s="62">
+        <v>2500</v>
       </c>
       <c r="E16" s="17">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F16" s="17">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="G16" s="17">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>802</v>
-      </c>
-      <c r="I16" s="17" t="s">
-        <v>803</v>
+        <v>798</v>
+      </c>
+      <c r="I16" s="62" t="s">
+        <v>674</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>629</v>
+        <v>643</v>
       </c>
       <c r="K16" s="17" t="s">
-        <v>691</v>
-      </c>
-      <c r="L16" s="17"/>
+        <v>642</v>
+      </c>
+      <c r="L16" s="62" t="s">
+        <v>2195</v>
+      </c>
       <c r="M16" s="17"/>
       <c r="N16" s="17"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>804</v>
+        <v>799</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -25275,16 +25312,16 @@
         <v>4</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="I17" s="17" t="s">
-        <v>705</v>
+        <v>721</v>
       </c>
       <c r="J17" s="17" t="s">
-        <v>805</v>
+        <v>661</v>
       </c>
       <c r="K17" s="17" t="s">
-        <v>806</v>
+        <v>800</v>
       </c>
       <c r="L17" s="17"/>
       <c r="M17" s="17"/>
@@ -25292,7 +25329,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>807</v>
+        <v>801</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -25304,7 +25341,7 @@
         <v>10000</v>
       </c>
       <c r="E18" s="17">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F18" s="17">
         <v>50</v>
@@ -25313,284 +25350,278 @@
         <v>4</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>786</v>
+        <v>802</v>
       </c>
       <c r="I18" s="17" t="s">
-        <v>732</v>
+        <v>803</v>
       </c>
       <c r="J18" s="17" t="s">
-        <v>764</v>
+        <v>629</v>
       </c>
       <c r="K18" s="17" t="s">
-        <v>808</v>
+        <v>691</v>
       </c>
       <c r="L18" s="17"/>
       <c r="M18" s="17"/>
       <c r="N18" s="17"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
-        <v>809</v>
-      </c>
-      <c r="B19" s="17">
+      <c r="A19" t="s">
+        <v>804</v>
+      </c>
+      <c r="B19">
         <v>0</v>
       </c>
-      <c r="C19" s="17">
-        <v>2</v>
-      </c>
-      <c r="D19" s="17">
-        <v>2500</v>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>10000</v>
       </c>
       <c r="E19" s="17">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="F19" s="17">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G19" s="17">
         <v>4</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="I19" s="17" t="s">
-        <v>810</v>
+        <v>705</v>
       </c>
       <c r="J19" s="17" t="s">
-        <v>811</v>
+        <v>805</v>
       </c>
       <c r="K19" s="17" t="s">
-        <v>812</v>
+        <v>806</v>
       </c>
       <c r="L19" s="17"/>
       <c r="M19" s="17"/>
       <c r="N19" s="17"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>813</v>
-      </c>
-      <c r="B20">
+      <c r="A20" s="8" t="s">
+        <v>2153</v>
+      </c>
+      <c r="B20" s="8">
         <v>0</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="8">
         <v>1</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="8">
         <v>10000</v>
       </c>
-      <c r="E20" s="17">
-        <v>35</v>
-      </c>
-      <c r="F20" s="17">
-        <v>70</v>
-      </c>
-      <c r="G20" s="17">
-        <v>4</v>
-      </c>
-      <c r="H20" s="17" t="s">
+      <c r="E20" s="13">
+        <v>15</v>
+      </c>
+      <c r="F20" s="13">
+        <v>50</v>
+      </c>
+      <c r="G20" s="8">
+        <v>3</v>
+      </c>
+      <c r="H20" s="8" t="s">
         <v>777</v>
       </c>
-      <c r="I20" s="17" t="s">
-        <v>739</v>
-      </c>
-      <c r="J20" s="17" t="s">
-        <v>1684</v>
-      </c>
-      <c r="K20" s="17" t="s">
-        <v>814</v>
-      </c>
-      <c r="L20" s="17"/>
-      <c r="M20" s="17"/>
-      <c r="N20" s="17"/>
+      <c r="I20" s="8" t="s">
+        <v>1070</v>
+      </c>
+      <c r="J20" t="s">
+        <v>796</v>
+      </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>815</v>
+      <c r="A21" s="8" t="s">
+        <v>2205</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="8">
         <v>1</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="8">
         <v>10000</v>
       </c>
-      <c r="E21" s="17">
-        <v>35</v>
-      </c>
-      <c r="F21" s="17">
-        <v>70</v>
-      </c>
-      <c r="G21" s="17">
+      <c r="E21" s="13">
+        <v>15</v>
+      </c>
+      <c r="F21" s="13">
+        <v>50</v>
+      </c>
+      <c r="G21" s="8">
         <v>4</v>
       </c>
-      <c r="H21" s="17" t="s">
-        <v>777</v>
-      </c>
-      <c r="I21" s="17" t="s">
-        <v>810</v>
-      </c>
-      <c r="J21" s="17" t="s">
-        <v>621</v>
-      </c>
-      <c r="K21" s="17" t="s">
-        <v>816</v>
-      </c>
-      <c r="L21" s="17"/>
-      <c r="M21" s="17"/>
-      <c r="N21" s="17"/>
+      <c r="H21" s="8" t="s">
+        <v>2206</v>
+      </c>
+      <c r="I21" t="s">
+        <v>2188</v>
+      </c>
+      <c r="J21" t="s">
+        <v>2207</v>
+      </c>
+      <c r="K21" t="s">
+        <v>688</v>
+      </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>817</v>
-      </c>
-      <c r="B22">
+      <c r="A22" s="2" t="s">
+        <v>1680</v>
+      </c>
+      <c r="B22" s="2">
         <v>0</v>
       </c>
-      <c r="C22" s="17">
-        <v>2</v>
-      </c>
-      <c r="D22" s="17">
-        <v>2500</v>
-      </c>
-      <c r="E22" s="17">
-        <v>40</v>
-      </c>
-      <c r="F22" s="17">
-        <v>100</v>
-      </c>
-      <c r="G22" s="17">
-        <v>3</v>
-      </c>
-      <c r="H22" s="17" t="s">
-        <v>779</v>
-      </c>
-      <c r="I22" s="17" t="s">
-        <v>818</v>
-      </c>
-      <c r="J22" s="17" t="s">
-        <v>805</v>
-      </c>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17"/>
-      <c r="N22" s="17"/>
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2">
+        <v>10000</v>
+      </c>
+      <c r="E22" s="9">
+        <v>20</v>
+      </c>
+      <c r="F22" s="9">
+        <v>50</v>
+      </c>
+      <c r="G22" s="2">
+        <v>4</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>1683</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>859</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>692</v>
+      </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>819</v>
+        <v>807</v>
       </c>
       <c r="B23">
         <v>0</v>
       </c>
-      <c r="C23" s="17">
-        <v>3</v>
-      </c>
-      <c r="D23" s="17">
-        <v>250</v>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>10000</v>
       </c>
       <c r="E23" s="17">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="F23" s="17">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G23" s="17">
         <v>4</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>777</v>
+        <v>786</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>643</v>
+        <v>732</v>
       </c>
       <c r="J23" s="17" t="s">
-        <v>820</v>
+        <v>764</v>
       </c>
       <c r="K23" s="17" t="s">
-        <v>721</v>
+        <v>808</v>
       </c>
       <c r="L23" s="17"/>
       <c r="M23" s="17"/>
       <c r="N23" s="17"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>821</v>
-      </c>
-      <c r="B24">
+      <c r="A24" s="17" t="s">
+        <v>809</v>
+      </c>
+      <c r="B24" s="17">
         <v>0</v>
       </c>
-      <c r="C24">
-        <v>4</v>
-      </c>
-      <c r="D24">
-        <v>50</v>
+      <c r="C24" s="17">
+        <v>2</v>
+      </c>
+      <c r="D24" s="17">
+        <v>2500</v>
       </c>
       <c r="E24" s="17">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="F24" s="17">
         <v>100</v>
       </c>
-      <c r="G24">
-        <v>6</v>
-      </c>
-      <c r="H24" t="s">
-        <v>822</v>
-      </c>
-      <c r="I24" t="s">
-        <v>621</v>
-      </c>
-      <c r="J24" t="s">
-        <v>691</v>
-      </c>
-      <c r="K24" t="s">
-        <v>796</v>
-      </c>
-      <c r="L24" t="s">
-        <v>823</v>
-      </c>
+      <c r="G24" s="17">
+        <v>4</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>777</v>
+      </c>
+      <c r="I24" s="17" t="s">
+        <v>810</v>
+      </c>
+      <c r="J24" s="17" t="s">
+        <v>811</v>
+      </c>
+      <c r="K24" s="17" t="s">
+        <v>812</v>
+      </c>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="17"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>824</v>
+        <v>813</v>
       </c>
       <c r="B25">
         <v>0</v>
       </c>
-      <c r="C25" s="17">
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>10000</v>
+      </c>
+      <c r="E25" s="17">
+        <v>35</v>
+      </c>
+      <c r="F25" s="17">
+        <v>70</v>
+      </c>
+      <c r="G25" s="17">
         <v>4</v>
       </c>
-      <c r="D25" s="17">
-        <v>50</v>
-      </c>
-      <c r="E25" s="17">
-        <v>45</v>
-      </c>
-      <c r="F25" s="17">
-        <v>100</v>
-      </c>
-      <c r="G25" s="17">
-        <v>2</v>
-      </c>
       <c r="H25" s="17" t="s">
-        <v>825</v>
+        <v>777</v>
       </c>
       <c r="I25" s="17" t="s">
-        <v>826</v>
-      </c>
-      <c r="J25" s="17"/>
-      <c r="K25" s="17"/>
+        <v>739</v>
+      </c>
+      <c r="J25" s="17" t="s">
+        <v>1684</v>
+      </c>
+      <c r="K25" s="17" t="s">
+        <v>814</v>
+      </c>
       <c r="L25" s="17"/>
       <c r="M25" s="17"/>
       <c r="N25" s="17"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>827</v>
+        <v>815</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -25602,25 +25633,25 @@
         <v>10000</v>
       </c>
       <c r="E26" s="17">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="F26" s="17">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="G26" s="17">
         <v>4</v>
       </c>
       <c r="H26" s="17" t="s">
-        <v>773</v>
+        <v>777</v>
       </c>
       <c r="I26" s="17" t="s">
-        <v>732</v>
+        <v>810</v>
       </c>
       <c r="J26" s="17" t="s">
-        <v>765</v>
+        <v>621</v>
       </c>
       <c r="K26" s="17" t="s">
-        <v>764</v>
+        <v>816</v>
       </c>
       <c r="L26" s="17"/>
       <c r="M26" s="17"/>
@@ -25628,19 +25659,19 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>828</v>
+        <v>817</v>
       </c>
       <c r="B27">
         <v>0</v>
       </c>
       <c r="C27" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D27" s="17">
-        <v>10000</v>
+        <v>2500</v>
       </c>
       <c r="E27" s="17">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F27" s="17">
         <v>100</v>
@@ -25649,114 +25680,110 @@
         <v>3</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>775</v>
+        <v>779</v>
       </c>
       <c r="I27" s="17" t="s">
-        <v>829</v>
+        <v>818</v>
       </c>
       <c r="J27" s="17" t="s">
-        <v>725</v>
-      </c>
-      <c r="K27" s="17" t="s">
-        <v>721</v>
-      </c>
+        <v>805</v>
+      </c>
+      <c r="K27" s="17"/>
       <c r="L27" s="17"/>
       <c r="M27" s="17"/>
       <c r="N27" s="17"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>830</v>
+        <v>819</v>
       </c>
       <c r="B28">
         <v>0</v>
       </c>
-      <c r="C28" s="17">
-        <v>3</v>
-      </c>
-      <c r="D28" s="17">
-        <v>250</v>
+      <c r="C28" s="62">
+        <v>2</v>
+      </c>
+      <c r="D28" s="62">
+        <v>2500</v>
       </c>
       <c r="E28" s="17">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F28" s="17">
         <v>100</v>
       </c>
       <c r="G28" s="17">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H28" s="17" t="s">
-        <v>786</v>
+        <v>777</v>
       </c>
       <c r="I28" s="17" t="s">
-        <v>661</v>
+        <v>643</v>
       </c>
       <c r="J28" s="17" t="s">
-        <v>629</v>
+        <v>820</v>
       </c>
       <c r="K28" s="17" t="s">
-        <v>750</v>
-      </c>
-      <c r="L28" s="17" t="s">
-        <v>831</v>
-      </c>
+        <v>721</v>
+      </c>
+      <c r="L28" s="17"/>
       <c r="M28" s="17"/>
       <c r="N28" s="17"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>832</v>
+        <v>821</v>
       </c>
       <c r="B29">
         <v>0</v>
       </c>
-      <c r="C29" s="17">
-        <v>1</v>
-      </c>
-      <c r="D29" s="17">
-        <v>10000</v>
+      <c r="C29" s="62">
+        <v>3</v>
+      </c>
+      <c r="D29" s="62">
+        <v>250</v>
       </c>
       <c r="E29" s="17">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F29" s="17">
         <v>100</v>
       </c>
-      <c r="G29" s="17">
-        <v>4</v>
-      </c>
-      <c r="H29" s="17" t="s">
-        <v>833</v>
-      </c>
-      <c r="I29" s="17" t="s">
-        <v>729</v>
-      </c>
-      <c r="J29" s="17" t="s">
-        <v>747</v>
-      </c>
-      <c r="K29" s="17" t="s">
-        <v>705</v>
-      </c>
-      <c r="L29" s="17"/>
-      <c r="M29" s="17"/>
-      <c r="N29" s="17"/>
+      <c r="G29">
+        <v>6</v>
+      </c>
+      <c r="H29" t="s">
+        <v>822</v>
+      </c>
+      <c r="I29" t="s">
+        <v>621</v>
+      </c>
+      <c r="J29" t="s">
+        <v>691</v>
+      </c>
+      <c r="K29" t="s">
+        <v>796</v>
+      </c>
+      <c r="L29" t="s">
+        <v>823</v>
+      </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>834</v>
+        <v>824</v>
       </c>
       <c r="B30">
         <v>0</v>
       </c>
-      <c r="C30" s="17">
-        <v>1</v>
-      </c>
-      <c r="D30" s="17">
-        <v>200555</v>
+      <c r="C30" s="62">
+        <v>3</v>
+      </c>
+      <c r="D30" s="62">
+        <v>250</v>
       </c>
       <c r="E30" s="17">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F30" s="17">
         <v>100</v>
@@ -25765,10 +25792,10 @@
         <v>2</v>
       </c>
       <c r="H30" s="17" t="s">
-        <v>835</v>
+        <v>825</v>
       </c>
       <c r="I30" s="17" t="s">
-        <v>836</v>
+        <v>826</v>
       </c>
       <c r="J30" s="17"/>
       <c r="K30" s="17"/>
@@ -25778,169 +25805,161 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>837</v>
+        <v>827</v>
       </c>
       <c r="B31">
         <v>0</v>
       </c>
-      <c r="C31" s="17">
-        <v>4</v>
-      </c>
-      <c r="D31" s="17">
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>10000</v>
+      </c>
+      <c r="E31" s="17">
         <v>50</v>
-      </c>
-      <c r="E31" s="17">
-        <v>70</v>
       </c>
       <c r="F31" s="17">
         <v>100</v>
       </c>
       <c r="G31" s="17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>786</v>
+        <v>773</v>
       </c>
       <c r="I31" s="17" t="s">
-        <v>688</v>
+        <v>732</v>
       </c>
       <c r="J31" s="17" t="s">
-        <v>1684</v>
-      </c>
-      <c r="K31" s="17"/>
+        <v>765</v>
+      </c>
+      <c r="K31" s="17" t="s">
+        <v>764</v>
+      </c>
       <c r="L31" s="17"/>
       <c r="M31" s="17"/>
       <c r="N31" s="17"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>838</v>
+        <v>828</v>
       </c>
       <c r="B32">
         <v>0</v>
       </c>
       <c r="C32" s="17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D32" s="17">
+        <v>10000</v>
+      </c>
+      <c r="E32" s="17">
         <v>50</v>
-      </c>
-      <c r="E32" s="17">
-        <v>70</v>
       </c>
       <c r="F32" s="17">
         <v>100</v>
       </c>
       <c r="G32" s="17">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>839</v>
+        <v>775</v>
       </c>
       <c r="I32" s="17" t="s">
-        <v>656</v>
+        <v>829</v>
       </c>
       <c r="J32" s="17" t="s">
-        <v>800</v>
+        <v>725</v>
       </c>
       <c r="K32" s="17" t="s">
-        <v>688</v>
-      </c>
-      <c r="L32" s="17" t="s">
-        <v>840</v>
-      </c>
-      <c r="M32" s="17" t="s">
-        <v>841</v>
-      </c>
+        <v>721</v>
+      </c>
+      <c r="L32" s="17"/>
+      <c r="M32" s="17"/>
       <c r="N32" s="17"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>842</v>
+        <v>830</v>
       </c>
       <c r="B33">
         <v>0</v>
       </c>
-      <c r="C33" s="17">
-        <v>4</v>
-      </c>
-      <c r="D33" s="17">
+      <c r="C33" s="62">
+        <v>2</v>
+      </c>
+      <c r="D33" s="62">
+        <v>2500</v>
+      </c>
+      <c r="E33" s="17">
         <v>50</v>
-      </c>
-      <c r="E33" s="17">
-        <v>70</v>
       </c>
       <c r="F33" s="17">
         <v>100</v>
       </c>
       <c r="G33" s="17">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H33" s="17" t="s">
-        <v>843</v>
+        <v>786</v>
       </c>
       <c r="I33" s="17" t="s">
-        <v>705</v>
+        <v>661</v>
       </c>
       <c r="J33" s="17" t="s">
-        <v>844</v>
+        <v>629</v>
       </c>
       <c r="K33" s="17" t="s">
-        <v>688</v>
+        <v>750</v>
       </c>
       <c r="L33" s="17" t="s">
-        <v>845</v>
-      </c>
-      <c r="M33" s="17" t="s">
-        <v>705</v>
-      </c>
+        <v>831</v>
+      </c>
+      <c r="M33" s="17"/>
       <c r="N33" s="17"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>846</v>
+        <v>832</v>
       </c>
       <c r="B34">
         <v>0</v>
       </c>
       <c r="C34" s="17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D34" s="17">
+        <v>10000</v>
+      </c>
+      <c r="E34" s="17">
         <v>50</v>
-      </c>
-      <c r="E34" s="17">
-        <v>70</v>
       </c>
       <c r="F34" s="17">
         <v>100</v>
       </c>
       <c r="G34" s="17">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H34" s="17" t="s">
-        <v>847</v>
+        <v>833</v>
       </c>
       <c r="I34" s="17" t="s">
-        <v>848</v>
+        <v>729</v>
       </c>
       <c r="J34" s="17" t="s">
-        <v>691</v>
+        <v>747</v>
       </c>
       <c r="K34" s="17" t="s">
-        <v>1684</v>
-      </c>
-      <c r="L34" s="17" t="s">
-        <v>656</v>
-      </c>
-      <c r="M34" s="17" t="s">
-        <v>2195</v>
-      </c>
+        <v>705</v>
+      </c>
+      <c r="L34" s="17"/>
+      <c r="M34" s="17"/>
       <c r="N34" s="17"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>849</v>
+        <v>834</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -25952,23 +25971,21 @@
         <v>10000</v>
       </c>
       <c r="E35" s="17">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="F35" s="17">
         <v>100</v>
       </c>
       <c r="G35" s="17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>850</v>
+        <v>835</v>
       </c>
       <c r="I35" s="17" t="s">
-        <v>810</v>
-      </c>
-      <c r="J35" s="17" t="s">
-        <v>851</v>
-      </c>
+        <v>836</v>
+      </c>
+      <c r="J35" s="17"/>
       <c r="K35" s="17"/>
       <c r="L35" s="17"/>
       <c r="M35" s="17"/>
@@ -25976,386 +25993,589 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>852</v>
+        <v>837</v>
       </c>
       <c r="B36">
         <v>0</v>
       </c>
-      <c r="C36">
-        <v>4</v>
-      </c>
-      <c r="D36">
-        <v>50</v>
+      <c r="C36" s="62">
+        <v>3</v>
+      </c>
+      <c r="D36" s="62">
+        <v>250</v>
       </c>
       <c r="E36" s="17">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="F36" s="17">
         <v>100</v>
       </c>
       <c r="G36" s="17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H36" s="17" t="s">
-        <v>777</v>
+        <v>786</v>
       </c>
       <c r="I36" s="17" t="s">
-        <v>853</v>
+        <v>688</v>
       </c>
       <c r="J36" s="17" t="s">
-        <v>854</v>
-      </c>
-      <c r="K36" s="17" t="s">
-        <v>788</v>
-      </c>
+        <v>1684</v>
+      </c>
+      <c r="K36" s="17"/>
       <c r="L36" s="17"/>
       <c r="M36" s="17"/>
       <c r="N36" s="17"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>855</v>
+        <v>838</v>
       </c>
       <c r="B37">
         <v>0</v>
       </c>
-      <c r="C37">
-        <v>4</v>
-      </c>
-      <c r="D37">
-        <v>50</v>
+      <c r="C37" s="62">
+        <v>3</v>
+      </c>
+      <c r="D37" s="62">
+        <v>250</v>
       </c>
       <c r="E37" s="17">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="F37" s="17">
         <v>100</v>
       </c>
-      <c r="G37">
-        <v>4</v>
-      </c>
-      <c r="H37" t="s">
-        <v>777</v>
-      </c>
-      <c r="I37" t="s">
-        <v>752</v>
-      </c>
-      <c r="J37" t="s">
-        <v>856</v>
-      </c>
-      <c r="K37" t="s">
-        <v>790</v>
-      </c>
+      <c r="G37" s="17">
+        <v>6</v>
+      </c>
+      <c r="H37" s="17" t="s">
+        <v>839</v>
+      </c>
+      <c r="I37" s="17" t="s">
+        <v>656</v>
+      </c>
+      <c r="J37" s="17" t="s">
+        <v>800</v>
+      </c>
+      <c r="K37" s="17" t="s">
+        <v>688</v>
+      </c>
+      <c r="L37" s="17" t="s">
+        <v>840</v>
+      </c>
+      <c r="M37" s="17" t="s">
+        <v>841</v>
+      </c>
+      <c r="N37" s="17"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>857</v>
+        <v>842</v>
       </c>
       <c r="B38">
         <v>0</v>
       </c>
-      <c r="C38">
-        <v>4</v>
-      </c>
-      <c r="D38">
-        <v>50</v>
+      <c r="C38" s="62">
+        <v>3</v>
+      </c>
+      <c r="D38" s="62">
+        <v>250</v>
       </c>
       <c r="E38" s="17">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="F38" s="17">
         <v>100</v>
       </c>
-      <c r="G38">
-        <v>4</v>
-      </c>
-      <c r="H38" t="s">
-        <v>777</v>
-      </c>
-      <c r="I38" t="s">
-        <v>858</v>
-      </c>
-      <c r="J38" t="s">
-        <v>859</v>
-      </c>
-      <c r="K38" t="s">
-        <v>794</v>
-      </c>
+      <c r="G38" s="17">
+        <v>6</v>
+      </c>
+      <c r="H38" s="17" t="s">
+        <v>843</v>
+      </c>
+      <c r="I38" s="17" t="s">
+        <v>705</v>
+      </c>
+      <c r="J38" s="17" t="s">
+        <v>844</v>
+      </c>
+      <c r="K38" s="17" t="s">
+        <v>688</v>
+      </c>
+      <c r="L38" s="17" t="s">
+        <v>845</v>
+      </c>
+      <c r="M38" s="17" t="s">
+        <v>705</v>
+      </c>
+      <c r="N38" s="17"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>860</v>
+        <v>846</v>
       </c>
       <c r="B39">
         <v>0</v>
       </c>
-      <c r="C39" s="17">
-        <v>4</v>
-      </c>
-      <c r="D39" s="17">
-        <v>50</v>
+      <c r="C39" s="62">
+        <v>3</v>
+      </c>
+      <c r="D39" s="62">
+        <v>250</v>
       </c>
       <c r="E39" s="17">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="F39" s="17">
         <v>100</v>
       </c>
       <c r="G39" s="17">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H39" s="17" t="s">
-        <v>777</v>
+        <v>847</v>
       </c>
       <c r="I39" s="17" t="s">
-        <v>861</v>
-      </c>
-      <c r="J39" t="s">
-        <v>862</v>
-      </c>
-      <c r="K39" t="s">
-        <v>792</v>
-      </c>
+        <v>848</v>
+      </c>
+      <c r="J39" s="17" t="s">
+        <v>691</v>
+      </c>
+      <c r="K39" s="17" t="s">
+        <v>1684</v>
+      </c>
+      <c r="L39" s="17" t="s">
+        <v>656</v>
+      </c>
+      <c r="M39" s="17" t="s">
+        <v>2195</v>
+      </c>
+      <c r="N39" s="17"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>863</v>
-      </c>
-      <c r="B40">
+      <c r="A40" s="8" t="s">
+        <v>2204</v>
+      </c>
+      <c r="B40" s="8">
         <v>0</v>
       </c>
-      <c r="C40">
-        <v>1</v>
-      </c>
-      <c r="D40">
-        <v>200555</v>
-      </c>
-      <c r="E40" t="s">
-        <v>864</v>
-      </c>
-      <c r="F40" t="s">
-        <v>864</v>
-      </c>
-      <c r="G40">
-        <v>2</v>
-      </c>
-      <c r="H40" t="s">
-        <v>865</v>
-      </c>
-      <c r="I40" t="s">
-        <v>692</v>
+      <c r="C40" s="62">
+        <v>3</v>
+      </c>
+      <c r="D40" s="62">
+        <v>250</v>
+      </c>
+      <c r="E40" s="13">
+        <v>70</v>
+      </c>
+      <c r="F40" s="13">
+        <v>100</v>
+      </c>
+      <c r="G40" s="8">
+        <v>6</v>
+      </c>
+      <c r="H40" s="8" t="s">
+        <v>833</v>
+      </c>
+      <c r="I40" s="8" t="s">
+        <v>752</v>
+      </c>
+      <c r="J40" t="s">
+        <v>2200</v>
+      </c>
+      <c r="K40" t="s">
+        <v>1333</v>
+      </c>
+      <c r="L40" t="s">
+        <v>1018</v>
+      </c>
+      <c r="M40" t="s">
+        <v>2208</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>1679</v>
+        <v>849</v>
       </c>
       <c r="B41">
         <v>0</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="62">
+        <v>2</v>
+      </c>
+      <c r="D41" s="62">
+        <v>2500</v>
+      </c>
+      <c r="E41" s="17">
+        <v>85</v>
+      </c>
+      <c r="F41" s="17">
+        <v>100</v>
+      </c>
+      <c r="G41" s="17">
+        <v>3</v>
+      </c>
+      <c r="H41" s="17" t="s">
+        <v>850</v>
+      </c>
+      <c r="I41" s="17" t="s">
+        <v>810</v>
+      </c>
+      <c r="J41" s="17" t="s">
+        <v>851</v>
+      </c>
+      <c r="K41" s="17"/>
+      <c r="L41" s="17"/>
+      <c r="M41" s="17"/>
+      <c r="N41" s="17"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>852</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>4</v>
+      </c>
+      <c r="D42">
+        <v>50</v>
+      </c>
+      <c r="E42" s="17">
+        <v>90</v>
+      </c>
+      <c r="F42" s="17">
+        <v>100</v>
+      </c>
+      <c r="G42" s="17">
+        <v>4</v>
+      </c>
+      <c r="H42" s="17" t="s">
+        <v>777</v>
+      </c>
+      <c r="I42" s="17" t="s">
+        <v>853</v>
+      </c>
+      <c r="J42" s="17" t="s">
+        <v>854</v>
+      </c>
+      <c r="K42" s="17" t="s">
+        <v>788</v>
+      </c>
+      <c r="L42" s="17"/>
+      <c r="M42" s="17"/>
+      <c r="N42" s="17"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>855</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>4</v>
+      </c>
+      <c r="D43">
+        <v>50</v>
+      </c>
+      <c r="E43" s="17">
+        <v>90</v>
+      </c>
+      <c r="F43" s="17">
+        <v>100</v>
+      </c>
+      <c r="G43">
+        <v>4</v>
+      </c>
+      <c r="H43" t="s">
+        <v>777</v>
+      </c>
+      <c r="I43" t="s">
+        <v>752</v>
+      </c>
+      <c r="J43" t="s">
+        <v>856</v>
+      </c>
+      <c r="K43" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>857</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>4</v>
+      </c>
+      <c r="D44">
+        <v>50</v>
+      </c>
+      <c r="E44" s="17">
+        <v>90</v>
+      </c>
+      <c r="F44" s="17">
+        <v>100</v>
+      </c>
+      <c r="G44">
+        <v>4</v>
+      </c>
+      <c r="H44" t="s">
+        <v>777</v>
+      </c>
+      <c r="I44" t="s">
+        <v>858</v>
+      </c>
+      <c r="J44" t="s">
+        <v>859</v>
+      </c>
+      <c r="K44" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>860</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45" s="17">
+        <v>4</v>
+      </c>
+      <c r="D45" s="17">
+        <v>50</v>
+      </c>
+      <c r="E45" s="17">
+        <v>90</v>
+      </c>
+      <c r="F45" s="17">
+        <v>100</v>
+      </c>
+      <c r="G45" s="17">
+        <v>4</v>
+      </c>
+      <c r="H45" s="17" t="s">
+        <v>777</v>
+      </c>
+      <c r="I45" s="17" t="s">
+        <v>861</v>
+      </c>
+      <c r="J45" t="s">
+        <v>862</v>
+      </c>
+      <c r="K45" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
+        <v>863</v>
+      </c>
+      <c r="B46" s="7">
+        <v>0</v>
+      </c>
+      <c r="C46" s="7">
         <v>1</v>
       </c>
-      <c r="D41">
+      <c r="D46" s="7">
         <v>10000</v>
       </c>
-      <c r="E41" s="17">
-        <v>5</v>
-      </c>
-      <c r="F41" s="17">
+      <c r="E46" s="7" t="s">
+        <v>864</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>864</v>
+      </c>
+      <c r="G46" s="7">
+        <v>2</v>
+      </c>
+      <c r="H46" s="7" t="s">
+        <v>865</v>
+      </c>
+      <c r="I46" s="7" t="s">
+        <v>692</v>
+      </c>
+      <c r="J46" s="7"/>
+      <c r="K46" s="7"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>2211</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>2</v>
+      </c>
+      <c r="D47">
+        <v>2500</v>
+      </c>
+      <c r="E47" s="17">
+        <v>50</v>
+      </c>
+      <c r="F47" s="17">
+        <v>100</v>
+      </c>
+      <c r="G47">
+        <v>4</v>
+      </c>
+      <c r="H47" s="17" t="s">
+        <v>2209</v>
+      </c>
+      <c r="I47" t="s">
+        <v>2210</v>
+      </c>
+      <c r="J47" t="s">
+        <v>2220</v>
+      </c>
+      <c r="K47" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>2212</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>4</v>
+      </c>
+      <c r="D48">
+        <v>50</v>
+      </c>
+      <c r="E48" s="17">
+        <v>70</v>
+      </c>
+      <c r="F48" s="17">
+        <v>100</v>
+      </c>
+      <c r="G48">
+        <v>3</v>
+      </c>
+      <c r="H48" t="s">
+        <v>777</v>
+      </c>
+      <c r="I48" s="17" t="s">
+        <v>2195</v>
+      </c>
+      <c r="J48" t="s">
+        <v>2219</v>
+      </c>
+      <c r="K48" t="s">
+        <v>2213</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>2214</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>2</v>
+      </c>
+      <c r="D49">
+        <v>2500</v>
+      </c>
+      <c r="E49" s="17">
+        <v>15</v>
+      </c>
+      <c r="F49" s="17">
+        <v>70</v>
+      </c>
+      <c r="G49">
+        <v>3</v>
+      </c>
+      <c r="H49" s="17" t="s">
+        <v>786</v>
+      </c>
+      <c r="I49" t="s">
+        <v>688</v>
+      </c>
+      <c r="J49" s="17" t="s">
+        <v>2195</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>2215</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>10000</v>
+      </c>
+      <c r="E50" s="17">
         <v>35</v>
       </c>
-      <c r="G41">
-        <v>4</v>
-      </c>
-      <c r="H41" t="s">
-        <v>1681</v>
-      </c>
-      <c r="I41" t="s">
-        <v>805</v>
-      </c>
-      <c r="J41" t="s">
-        <v>800</v>
-      </c>
-      <c r="K41" t="s">
-        <v>1682</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>1680</v>
-      </c>
-      <c r="B42" s="2">
+      <c r="F50" s="17">
+        <v>70</v>
+      </c>
+      <c r="G50">
+        <v>3</v>
+      </c>
+      <c r="H50" s="17" t="s">
+        <v>2209</v>
+      </c>
+      <c r="I50" t="s">
+        <v>2216</v>
+      </c>
+      <c r="J50" t="s">
+        <v>2217</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>2218</v>
+      </c>
+      <c r="B51">
         <v>0</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C51">
         <v>1</v>
       </c>
-      <c r="D42" s="2">
+      <c r="D51">
         <v>10000</v>
       </c>
-      <c r="E42" s="9">
-        <v>20</v>
-      </c>
-      <c r="F42" s="9">
-        <v>50</v>
-      </c>
-      <c r="G42" s="2">
-        <v>4</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>1683</v>
-      </c>
-      <c r="I42" s="2" t="s">
-        <v>661</v>
-      </c>
-      <c r="J42" s="2" t="s">
-        <v>859</v>
-      </c>
-      <c r="K42" s="2" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
-        <v>2152</v>
-      </c>
-      <c r="B43" s="8">
-        <v>0</v>
-      </c>
-      <c r="C43" s="8">
-        <v>1</v>
-      </c>
-      <c r="D43" s="8">
-        <v>10000</v>
-      </c>
-      <c r="E43" s="13">
-        <v>0</v>
-      </c>
-      <c r="F43" s="13">
-        <v>20</v>
-      </c>
-      <c r="G43" s="8">
-        <v>2</v>
-      </c>
-      <c r="H43" s="8" t="s">
-        <v>777</v>
-      </c>
-      <c r="I43" s="8" t="s">
-        <v>796</v>
-      </c>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="s">
-        <v>2153</v>
-      </c>
-      <c r="B44" s="8">
-        <v>0</v>
-      </c>
-      <c r="C44" s="8">
-        <v>1</v>
-      </c>
-      <c r="D44" s="8">
-        <v>10000</v>
-      </c>
-      <c r="E44" s="13">
-        <v>15</v>
-      </c>
-      <c r="F44" s="13">
-        <v>50</v>
-      </c>
-      <c r="G44" s="8">
+      <c r="E51" s="17">
+        <v>10</v>
+      </c>
+      <c r="F51" s="17">
+        <v>40</v>
+      </c>
+      <c r="G51">
         <v>3</v>
       </c>
-      <c r="H44" s="8" t="s">
-        <v>777</v>
-      </c>
-      <c r="I44" s="8" t="s">
-        <v>1070</v>
-      </c>
-      <c r="J44" t="s">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
-        <v>2204</v>
-      </c>
-      <c r="B45" s="8">
-        <v>0</v>
-      </c>
-      <c r="C45" s="8">
-        <v>4</v>
-      </c>
-      <c r="D45" s="8">
-        <v>50</v>
-      </c>
-      <c r="E45" s="13">
-        <v>70</v>
-      </c>
-      <c r="F45" s="13">
-        <v>100</v>
-      </c>
-      <c r="G45" s="8">
-        <v>6</v>
-      </c>
-      <c r="H45" s="8" t="s">
-        <v>833</v>
-      </c>
-      <c r="I45" s="8" t="s">
-        <v>752</v>
-      </c>
-      <c r="J45" t="s">
-        <v>2200</v>
-      </c>
-      <c r="K45" t="s">
-        <v>1333</v>
-      </c>
-      <c r="L45" t="s">
-        <v>1018</v>
-      </c>
-      <c r="M45" t="s">
-        <v>2208</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="8" t="s">
-        <v>2205</v>
-      </c>
-      <c r="B46">
-        <v>0</v>
-      </c>
-      <c r="C46" s="8">
-        <v>1</v>
-      </c>
-      <c r="D46" s="8">
-        <v>10000</v>
-      </c>
-      <c r="E46" s="13">
-        <v>15</v>
-      </c>
-      <c r="F46" s="13">
-        <v>50</v>
-      </c>
-      <c r="G46" s="8">
-        <v>4</v>
-      </c>
-      <c r="H46" s="8" t="s">
-        <v>2206</v>
-      </c>
-      <c r="I46" t="s">
-        <v>2188</v>
-      </c>
-      <c r="J46" t="s">
-        <v>2207</v>
-      </c>
-      <c r="K46" t="s">
-        <v>688</v>
+      <c r="H51" s="17" t="s">
+        <v>779</v>
+      </c>
+      <c r="I51" t="s">
+        <v>747</v>
+      </c>
+      <c r="J51" t="s">
+        <v>1005</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:N1" xr:uid="{53C31A42-FE05-418B-83B3-86861291C9F6}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:N46">
+      <sortCondition ref="E1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -26368,8 +26588,8 @@
   </sheetPr>
   <dimension ref="A1:P161"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="I102" sqref="I102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32285,7 +32505,7 @@
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
affix and spell speed stuff
</commit_message>
<xml_diff>
--- a/INFO D.xlsx
+++ b/INFO D.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kelvin\Documents\GitHub\Craft-to-Exile-Dissonance-Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{296AD62F-C770-4D4E-8E38-88B45FC67041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4831FDB4-5956-437B-9539-6B4689EB4661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="525" windowWidth="29040" windowHeight="16440" tabRatio="680" firstSheet="6" activeTab="14" xr2:uid="{52F6E08D-EA9B-4E8E-A88E-E860D0D32EA0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" tabRatio="680" firstSheet="7" activeTab="22" xr2:uid="{52F6E08D-EA9B-4E8E-A88E-E860D0D32EA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Overworld" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,7 @@
     <sheet name="Skill Tree Perks" sheetId="25" r:id="rId20"/>
     <sheet name="Talent Perks" sheetId="22" r:id="rId21"/>
     <sheet name="MineColonies Research" sheetId="23" r:id="rId22"/>
+    <sheet name="Physical Tree" sheetId="30" r:id="rId23"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">'Affixes (cont.)'!$A$1:$J$1</definedName>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4746" uniqueCount="2595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4785" uniqueCount="2634">
   <si>
     <t>Quest</t>
   </si>
@@ -7846,6 +7847,463 @@
   </si>
   <si>
     <t>increased_proj_speed_flat</t>
+  </si>
+  <si>
+    <t>Passives</t>
+  </si>
+  <si>
+    <t>Raging Dragon Linker</t>
+  </si>
+  <si>
+    <t>Empowering Finisher</t>
+  </si>
+  <si>
+    <t>Elemental Vengeance Finisher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit Drain Linker </t>
+  </si>
+  <si>
+    <t>(nature dmg, heal self hp, mana, energy)</t>
+  </si>
+  <si>
+    <t>(fire/lightn projectile)</t>
+  </si>
+  <si>
+    <t>(all elements, big aoe)</t>
+  </si>
+  <si>
+    <t>(aoe, grant many stacks of empower to allies)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Elemental Strike</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (all elements)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sweeping Strike</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (aoe)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Goading Strike</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (aoe, taunt)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Debilitating Strike</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (lowrs dmg, spd)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Piercing Strike</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (lowers def)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Empower</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (inc. dmg)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Enlighten</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (inc. regen, cdr, cast rate)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Triple Attack Linker</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (3x hit)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Earthen Smash Finisher</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (aoe nature dmg, buff ally def)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Flowing River Linker</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (2x frost hit, heal allies)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Power Form</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (att give empower to nearby allies)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Wisdom Form</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (att give wisdom to nearby allies)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Power Form Rush</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (expend power form buff to grant many stacks of empower, long cooldown)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Wisdom Form Rush</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (expend wisdom form buff to grant many stacks of enlighten, long cooldown)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Omnislash Finisher</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (really high dmg rapid attacks)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Anti-gravity Finisher</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (aoe, make enemies levitate)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Rallying Sweep Linker</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (aoe dmg, buff allies with speed and dmg)</t>
+    </r>
+  </si>
+  <si>
+    <t>"strikes" grant the attacker</t>
+  </si>
+  <si>
+    <t>a combo starter stack</t>
+  </si>
+  <si>
+    <t>linker spells REQUIRE a combo</t>
+  </si>
+  <si>
+    <t>starter stack to be cast, and grant</t>
+  </si>
+  <si>
+    <t>the attacker a combo extender stack</t>
+  </si>
+  <si>
+    <t>finishers REQUIRE a combo</t>
+  </si>
+  <si>
+    <t>extender stack to be cast</t>
+  </si>
+  <si>
+    <t>they also expend the combo starter</t>
+  </si>
+  <si>
+    <t>stack</t>
+  </si>
+  <si>
+    <t>they also expend the combo</t>
+  </si>
+  <si>
+    <t>extender stack</t>
+  </si>
+  <si>
+    <t>buffs</t>
+  </si>
+  <si>
+    <t>PHYSICAL TREE</t>
   </si>
 </sst>
 </file>
@@ -8133,7 +8591,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -8202,6 +8660,12 @@
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -27847,7 +28311,7 @@
   </sheetPr>
   <dimension ref="A1:P164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+    <sheetView topLeftCell="A73" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -42752,6 +43216,272 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6B49BBD-0DB4-4D92-9AC0-32DC0162AF4D}">
+  <dimension ref="B2:J31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="10" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>2633</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="73">
+        <v>50</v>
+      </c>
+      <c r="D4" s="68"/>
+      <c r="F4" s="69"/>
+      <c r="H4" s="71" t="s">
+        <v>2618</v>
+      </c>
+      <c r="J4" s="72"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="73"/>
+      <c r="D5" s="68"/>
+      <c r="F5" s="69"/>
+      <c r="H5" s="71"/>
+      <c r="J5" s="72"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="73">
+        <v>40</v>
+      </c>
+      <c r="D6" s="68"/>
+      <c r="F6" s="69"/>
+      <c r="H6" s="66" t="s">
+        <v>2598</v>
+      </c>
+      <c r="J6" s="72" t="s">
+        <v>2617</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="73"/>
+      <c r="D7" s="68"/>
+      <c r="F7" s="69"/>
+      <c r="H7" s="71" t="s">
+        <v>2602</v>
+      </c>
+      <c r="J7" s="72"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="73">
+        <v>30</v>
+      </c>
+      <c r="D8" s="68" t="s">
+        <v>2604</v>
+      </c>
+      <c r="F8" s="70" t="s">
+        <v>2599</v>
+      </c>
+      <c r="H8" s="71" t="s">
+        <v>2619</v>
+      </c>
+      <c r="J8" s="72"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="73"/>
+      <c r="D9" s="68"/>
+      <c r="F9" s="69" t="s">
+        <v>2600</v>
+      </c>
+      <c r="H9" s="71"/>
+      <c r="J9" s="72"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="73">
+        <v>25</v>
+      </c>
+      <c r="D10" s="68"/>
+      <c r="F10" s="69" t="s">
+        <v>2620</v>
+      </c>
+      <c r="H10" s="71"/>
+      <c r="J10" s="72" t="s">
+        <v>2616</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="73"/>
+      <c r="D11" s="68"/>
+      <c r="F11" s="69"/>
+      <c r="H11" s="71"/>
+      <c r="J11" s="72"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="73">
+        <v>20</v>
+      </c>
+      <c r="D12" s="68" t="s">
+        <v>2605</v>
+      </c>
+      <c r="F12" s="69"/>
+      <c r="H12" s="71"/>
+      <c r="J12" s="72"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="73"/>
+      <c r="D13" s="68"/>
+      <c r="F13" s="69"/>
+      <c r="H13" s="71"/>
+      <c r="J13" s="72"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="73">
+        <v>15</v>
+      </c>
+      <c r="D14" s="68" t="s">
+        <v>2606</v>
+      </c>
+      <c r="F14" s="70" t="s">
+        <v>2596</v>
+      </c>
+      <c r="H14" s="66" t="s">
+        <v>2597</v>
+      </c>
+      <c r="J14" s="72" t="s">
+        <v>2615</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="73"/>
+      <c r="D15" s="68"/>
+      <c r="F15" s="69" t="s">
+        <v>2601</v>
+      </c>
+      <c r="H15" s="71" t="s">
+        <v>2603</v>
+      </c>
+      <c r="J15" s="72"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="73">
+        <v>10</v>
+      </c>
+      <c r="D16" s="68" t="s">
+        <v>2607</v>
+      </c>
+      <c r="F16" s="69" t="s">
+        <v>2613</v>
+      </c>
+      <c r="H16" s="71"/>
+      <c r="J16" s="72"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="73"/>
+      <c r="D17" s="68"/>
+      <c r="F17" s="69"/>
+      <c r="H17" s="71"/>
+      <c r="J17" s="72"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="73">
+        <v>5</v>
+      </c>
+      <c r="D18" s="68"/>
+      <c r="F18" s="69"/>
+      <c r="H18" s="71"/>
+      <c r="J18" s="72" t="s">
+        <v>2614</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="73"/>
+      <c r="D19" s="68"/>
+      <c r="F19" s="69"/>
+      <c r="H19" s="71"/>
+      <c r="J19" s="72"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="73">
+        <v>1</v>
+      </c>
+      <c r="D20" s="68" t="s">
+        <v>2608</v>
+      </c>
+      <c r="F20" s="69" t="s">
+        <v>2611</v>
+      </c>
+      <c r="H20" s="71" t="s">
+        <v>2612</v>
+      </c>
+      <c r="J20" s="72"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="73"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="73" t="s">
+        <v>2595</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2609</v>
+      </c>
+      <c r="F22" t="s">
+        <v>2610</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D27" s="68" t="s">
+        <v>2621</v>
+      </c>
+      <c r="F27" s="69" t="s">
+        <v>2623</v>
+      </c>
+      <c r="H27" s="71" t="s">
+        <v>2626</v>
+      </c>
+      <c r="J27" s="72" t="s">
+        <v>2632</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>2622</v>
+      </c>
+      <c r="F28" t="s">
+        <v>2624</v>
+      </c>
+      <c r="H28" t="s">
+        <v>2627</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>2625</v>
+      </c>
+      <c r="H29" t="s">
+        <v>2630</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>2628</v>
+      </c>
+      <c r="H30" t="s">
+        <v>2631</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>2629</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B10869D-BB98-446E-A391-D8AB9A1D34DF}">
   <sheetPr>

</xml_diff>